<commit_message>
2good with O and G
</commit_message>
<xml_diff>
--- a/good_rbrush/keepingtabs_goodrbrush.xlsx
+++ b/good_rbrush/keepingtabs_goodrbrush.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinson_lab/Documents/RAD2/good_rbrush/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AD65345-88CB-E04B-9738-A27CB69A20A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D02D80F-CC0F-FE44-B97B-2EB240E31BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" xr2:uid="{91869BB1-4A8F-8E4D-BA74-EB15BB630210}"/>
+    <workbookView xWindow="5160" yWindow="2060" windowWidth="32820" windowHeight="19300" activeTab="1" xr2:uid="{91869BB1-4A8F-8E4D-BA74-EB15BB630210}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="with O and G" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="124">
   <si>
     <t>id</t>
   </si>
@@ -375,19 +376,58 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>removed from structure</t>
+  </si>
+  <si>
+    <t>C not S</t>
+  </si>
+  <si>
+    <t>S not C</t>
+  </si>
+  <si>
+    <t>MOB_EN_G_05</t>
+  </si>
+  <si>
+    <t>_G</t>
+  </si>
+  <si>
+    <t>MOB_EN_G_06</t>
+  </si>
+  <si>
+    <t>MOB_EN_G_07</t>
+  </si>
+  <si>
+    <t>SLV_EN_O_01</t>
+  </si>
+  <si>
+    <t>_O</t>
+  </si>
+  <si>
+    <t>SLV_EN_O_03</t>
+  </si>
+  <si>
+    <t>SLV_EN_O_07</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -410,8 +450,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,19 +768,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0D48B9B-FC4B-BB4E-905C-2E41992A16AF}">
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="3" max="4" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -748,8 +790,11 @@
       <c r="C1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -759,8 +804,11 @@
       <c r="C2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -768,7 +816,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -776,15 +824,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -792,7 +846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -800,10 +854,13 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+      <c r="D7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -811,7 +868,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -819,7 +876,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -827,7 +884,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -835,7 +892,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -843,7 +900,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -851,7 +908,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -859,7 +916,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -867,7 +924,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -875,7 +932,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -883,7 +940,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -891,15 +948,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -907,7 +967,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -915,7 +975,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -923,7 +983,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -931,7 +991,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -939,7 +999,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -947,7 +1007,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -955,7 +1015,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -963,7 +1023,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -971,7 +1031,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -979,7 +1039,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -987,7 +1047,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -995,7 +1055,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1265,7 +1325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>72</v>
       </c>
@@ -1275,8 +1335,11 @@
       <c r="C65" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>73</v>
       </c>
@@ -1287,7 +1350,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -1295,7 +1358,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -1303,7 +1366,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -1311,7 +1374,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -1319,7 +1382,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>78</v>
       </c>
@@ -1327,7 +1390,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>79</v>
       </c>
@@ -1335,7 +1398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>80</v>
       </c>
@@ -1343,7 +1406,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>81</v>
       </c>
@@ -1351,7 +1414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -1359,7 +1422,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>83</v>
       </c>
@@ -1367,7 +1430,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>84</v>
       </c>
@@ -1375,7 +1438,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -1383,7 +1446,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>86</v>
       </c>
@@ -1391,7 +1454,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>87</v>
       </c>
@@ -1399,7 +1462,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>88</v>
       </c>
@@ -1407,7 +1470,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>89</v>
       </c>
@@ -1415,7 +1478,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>90</v>
       </c>
@@ -1423,7 +1486,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>91</v>
       </c>
@@ -1431,7 +1494,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>92</v>
       </c>
@@ -1439,7 +1502,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>93</v>
       </c>
@@ -1447,7 +1510,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>94</v>
       </c>
@@ -1455,7 +1518,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>95</v>
       </c>
@@ -1463,7 +1526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>96</v>
       </c>
@@ -1471,7 +1534,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>97</v>
       </c>
@@ -1479,7 +1542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>98</v>
       </c>
@@ -1487,7 +1550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>99</v>
       </c>
@@ -1495,7 +1558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>100</v>
       </c>
@@ -1503,7 +1566,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>101</v>
       </c>
@@ -1513,8 +1576,11 @@
       <c r="C94" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>102</v>
       </c>
@@ -1522,7 +1588,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>103</v>
       </c>
@@ -1576,6 +1642,1441 @@
       </c>
       <c r="B102" t="s">
         <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E48A005D-7026-4F40-B9E1-C7FFB83FE6D9}">
+  <dimension ref="A1:J101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I90" sqref="I90"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>111</v>
+      </c>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>68</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>70</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>72</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>76</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>77</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>84</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>86</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>87</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>88</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>89</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>90</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>91</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>92</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>93</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>94</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>95</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D96" t="s">
+        <v>111</v>
+      </c>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>96</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>97</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>98</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>99</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J100" s="1"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>100</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>